<commit_message>
First Fully Functional Build
All Fact Sheet .JS files have been created and added. Adjusted GUI by removing old funds that are no longer active.

Created IF statement that checks if data backups have "-brochure" backup and creates csv's accordingly.

Just about ready to go live and create installer
</commit_message>
<xml_diff>
--- a/assets/ChartBuilder/public/Data/Backups/Catalyst/ATR/atr.xlsx
+++ b/assets/ChartBuilder/public/Data/Backups/Catalyst/ATR/atr.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jacob\Dropbox (Catalyst Funds)\Marketing Team Files\Marketing Materials\AutoCharts&amp;Tables\Backup Files\Catalyst\ATR\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\Marketing Team Files\Marketing Materials\AutoCharts&amp;Tables\Backup Files\Catalyst\ATR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C650D1B3-E07C-431A-8107-ADB7BB565BBE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90FD6FF0-6123-421D-A8D2-E90C38BC3850}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28692" yWindow="-108" windowWidth="29016" windowHeight="15816" xr2:uid="{2098151C-B5D8-4999-8AAB-2D570887D6E5}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2098151C-B5D8-4999-8AAB-2D570887D6E5}"/>
   </bookViews>
   <sheets>
     <sheet name="ATR Back Up" sheetId="1" r:id="rId1"/>
@@ -586,20 +586,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7D5812C-CC04-4C23-9449-0357AB8DA747}">
   <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.109375" customWidth="1"/>
-    <col min="7" max="7" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.140625" customWidth="1"/>
+    <col min="7" max="7" width="8.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="27" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="39" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -622,122 +624,122 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="6">
-        <v>8.94</v>
+        <v>5.5</v>
       </c>
       <c r="C2" s="6">
-        <v>14.98</v>
+        <v>5.5</v>
       </c>
       <c r="D2" s="6">
-        <v>14.98</v>
+        <v>33.86</v>
       </c>
       <c r="E2" s="6">
-        <v>5.93</v>
+        <v>11.01</v>
       </c>
       <c r="F2" s="6">
-        <v>3.35</v>
+        <v>4.68</v>
       </c>
       <c r="G2" s="7">
-        <v>2.56</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+        <v>3.29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="3">
-        <v>8.73</v>
+        <v>5.39</v>
       </c>
       <c r="C3" s="3">
-        <v>14.05</v>
+        <v>5.39</v>
       </c>
       <c r="D3" s="3">
-        <v>14.05</v>
+        <v>32.92</v>
       </c>
       <c r="E3" s="3">
-        <v>5.1100000000000003</v>
+        <v>10.18</v>
       </c>
       <c r="F3" s="17">
-        <v>2.5</v>
+        <v>3.86</v>
       </c>
       <c r="G3" s="9">
-        <v>1.74</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+        <v>2.48</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="3">
-        <v>9.0299999999999994</v>
+        <v>5.61</v>
       </c>
       <c r="C4" s="3">
-        <v>15.28</v>
+        <v>5.61</v>
       </c>
       <c r="D4" s="3">
-        <v>15.28</v>
+        <v>34.25</v>
       </c>
       <c r="E4" s="3">
-        <v>6.18</v>
+        <v>11.28</v>
       </c>
       <c r="F4" s="3">
-        <v>3.58</v>
+        <v>4.95</v>
       </c>
       <c r="G4" s="9">
-        <v>2.75</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+        <v>3.49</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
         <v>9</v>
       </c>
       <c r="B5" s="4">
-        <v>12.15</v>
+        <v>6.17</v>
       </c>
       <c r="C5" s="4">
-        <v>18.399999999999999</v>
+        <v>6.17</v>
       </c>
       <c r="D5" s="4">
-        <v>18.399999999999999</v>
+        <v>56.35</v>
       </c>
       <c r="E5" s="4">
-        <v>14.18</v>
+        <v>16.78</v>
       </c>
       <c r="F5" s="4">
-        <v>15.22</v>
+        <v>16.29</v>
       </c>
       <c r="G5" s="11">
-        <v>13.19</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+        <v>13.69</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
         <v>12</v>
       </c>
       <c r="B6" s="13">
-        <v>2.67</v>
+        <v>-0.6</v>
       </c>
       <c r="C6" s="13">
-        <v>8.32</v>
+        <v>-0.6</v>
       </c>
       <c r="D6" s="13">
-        <v>8.32</v>
+        <v>26.14</v>
       </c>
       <c r="E6" s="13">
-        <v>3.87</v>
+        <v>8.86</v>
       </c>
       <c r="F6" s="13">
-        <v>2.13</v>
+        <v>3.45</v>
       </c>
       <c r="G6" s="14">
-        <v>1.61</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+        <v>2.37</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="15" t="s">
         <v>10</v>
       </c>
@@ -751,21 +753,21 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D3ADAAE-B783-4A94-9171-A2FBA92D4B10}">
   <sheetPr>
-    <tabColor rgb="FFC00000"/>
+    <tabColor rgb="FFFF0000"/>
   </sheetPr>
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22" bestFit="1" customWidth="1"/>
-    <col min="2" max="5" width="9.109375" style="16"/>
-    <col min="6" max="6" width="8.88671875" style="16"/>
-    <col min="7" max="7" width="15.6640625" style="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="5" width="9.140625" style="16"/>
+    <col min="6" max="6" width="8.85546875" style="16"/>
+    <col min="7" max="7" width="15.7109375" style="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="str">
         <f>'ATR Back Up'!A1</f>
         <v>Share Class/Benchmark</v>
@@ -798,166 +800,166 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="str">
         <f>'ATR Back Up'!A2</f>
         <v>Class A</v>
       </c>
       <c r="B2" s="16">
         <f>'ATR Back Up'!B2</f>
-        <v>8.94</v>
+        <v>5.5</v>
       </c>
       <c r="C2" s="16">
         <f>'ATR Back Up'!C2</f>
-        <v>14.98</v>
+        <v>5.5</v>
       </c>
       <c r="D2" s="16">
         <f>'ATR Back Up'!D2</f>
-        <v>14.98</v>
+        <v>33.86</v>
       </c>
       <c r="E2" s="16">
         <f>'ATR Back Up'!E2</f>
-        <v>5.93</v>
+        <v>11.01</v>
       </c>
       <c r="F2" s="16">
         <f>'ATR Back Up'!F2</f>
-        <v>3.35</v>
+        <v>4.68</v>
       </c>
       <c r="G2" s="16">
         <f>'ATR Back Up'!G2</f>
-        <v>2.56</v>
+        <v>3.29</v>
       </c>
       <c r="H2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="str">
         <f>'ATR Back Up'!A3</f>
         <v>Class C</v>
       </c>
       <c r="B3" s="16">
         <f>'ATR Back Up'!B3</f>
-        <v>8.73</v>
+        <v>5.39</v>
       </c>
       <c r="C3" s="16">
         <f>'ATR Back Up'!C3</f>
-        <v>14.05</v>
+        <v>5.39</v>
       </c>
       <c r="D3" s="16">
         <f>'ATR Back Up'!D3</f>
-        <v>14.05</v>
+        <v>32.92</v>
       </c>
       <c r="E3" s="16">
         <f>'ATR Back Up'!E3</f>
-        <v>5.1100000000000003</v>
+        <v>10.18</v>
       </c>
       <c r="F3" s="16">
         <f>'ATR Back Up'!F3</f>
-        <v>2.5</v>
+        <v>3.86</v>
       </c>
       <c r="G3" s="16">
         <f>'ATR Back Up'!G3</f>
-        <v>1.74</v>
+        <v>2.48</v>
       </c>
       <c r="H3">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="str">
         <f>'ATR Back Up'!A4</f>
         <v>Class I</v>
       </c>
       <c r="B4" s="16">
         <f>'ATR Back Up'!B4</f>
-        <v>9.0299999999999994</v>
+        <v>5.61</v>
       </c>
       <c r="C4" s="16">
         <f>'ATR Back Up'!C4</f>
-        <v>15.28</v>
+        <v>5.61</v>
       </c>
       <c r="D4" s="16">
         <f>'ATR Back Up'!D4</f>
-        <v>15.28</v>
+        <v>34.25</v>
       </c>
       <c r="E4" s="16">
         <f>'ATR Back Up'!E4</f>
-        <v>6.18</v>
+        <v>11.28</v>
       </c>
       <c r="F4" s="16">
         <f>'ATR Back Up'!F4</f>
-        <v>3.58</v>
+        <v>4.95</v>
       </c>
       <c r="G4" s="16">
         <f>'ATR Back Up'!G4</f>
-        <v>2.75</v>
+        <v>3.49</v>
       </c>
       <c r="H4">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="str">
         <f>'ATR Back Up'!A5</f>
         <v>S&amp;P 500 TR Index</v>
       </c>
       <c r="B5" s="16">
         <f>'ATR Back Up'!B5</f>
-        <v>12.15</v>
+        <v>6.17</v>
       </c>
       <c r="C5" s="16">
         <f>'ATR Back Up'!C5</f>
-        <v>18.399999999999999</v>
+        <v>6.17</v>
       </c>
       <c r="D5" s="16">
         <f>'ATR Back Up'!D5</f>
-        <v>18.399999999999999</v>
+        <v>56.35</v>
       </c>
       <c r="E5" s="16">
         <f>'ATR Back Up'!E5</f>
-        <v>14.18</v>
+        <v>16.78</v>
       </c>
       <c r="F5" s="16">
         <f>'ATR Back Up'!F5</f>
-        <v>15.22</v>
+        <v>16.29</v>
       </c>
       <c r="G5" s="16">
         <f>'ATR Back Up'!G5</f>
-        <v>13.19</v>
+        <v>13.69</v>
       </c>
       <c r="H5">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="str">
         <f>'ATR Back Up'!A6</f>
         <v>Class A w/ Sales Charge</v>
       </c>
       <c r="B6" s="16">
         <f>'ATR Back Up'!B6</f>
-        <v>2.67</v>
+        <v>-0.6</v>
       </c>
       <c r="C6" s="16">
         <f>'ATR Back Up'!C6</f>
-        <v>8.32</v>
+        <v>-0.6</v>
       </c>
       <c r="D6" s="16">
         <f>'ATR Back Up'!D6</f>
-        <v>8.32</v>
+        <v>26.14</v>
       </c>
       <c r="E6" s="16">
         <f>'ATR Back Up'!E6</f>
-        <v>3.87</v>
+        <v>8.86</v>
       </c>
       <c r="F6" s="16">
         <f>'ATR Back Up'!F6</f>
-        <v>2.13</v>
+        <v>3.45</v>
       </c>
       <c r="G6" s="16">
         <f>'ATR Back Up'!G6</f>
-        <v>1.61</v>
+        <v>2.37</v>
       </c>
       <c r="H6">
         <v>5</v>

</xml_diff>